<commit_message>
Added NFL 2019 Divisional Round forecasts
</commit_message>
<xml_diff>
--- a/NFL2019/Weekly Forecasts/WeekWC2019Matrix.xlsx
+++ b/NFL2019/Weekly Forecasts/WeekWC2019Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MerrerPredictifier\MerrerPredictifier\NFL2019\Weekly Forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C34D61B-C5DF-4B40-9DA3-7BE6FC8B50E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2655F9-F1FE-49F9-950C-E646527DE6CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,19 +735,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -831,6 +819,24 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -841,12 +847,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -894,7 +894,7 @@
       <sheetName val="SEA"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="E3">
@@ -907,17 +907,17 @@
       </sheetData>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1285,16 +1285,16 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="27"/>
+      <c r="I3" s="57"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
-      <c r="O3" s="28"/>
+      <c r="O3" s="26"/>
     </row>
     <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="24"/>
@@ -1303,16 +1303,16 @@
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="30"/>
+      <c r="I4" s="59"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
       <c r="M4" s="25"/>
       <c r="N4" s="25"/>
-      <c r="O4" s="28"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="24"/>
@@ -1321,16 +1321,16 @@
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="59"/>
+      <c r="I5" s="61"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
       <c r="M5" s="25"/>
       <c r="N5" s="25"/>
-      <c r="O5" s="28"/>
+      <c r="O5" s="26"/>
     </row>
     <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="24"/>
@@ -1339,16 +1339,16 @@
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="61"/>
+      <c r="I6" s="63"/>
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
       <c r="M6" s="25"/>
       <c r="N6" s="25"/>
-      <c r="O6" s="28"/>
+      <c r="O6" s="26"/>
     </row>
     <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="24"/>
@@ -1358,13 +1358,13 @@
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
-      <c r="I7" s="56"/>
+      <c r="I7" s="52"/>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
       <c r="N7" s="25"/>
-      <c r="O7" s="28"/>
+      <c r="O7" s="26"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="24"/>
@@ -1373,10 +1373,10 @@
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="53" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="25"/>
@@ -1384,7 +1384,7 @@
       <c r="L8" s="25"/>
       <c r="M8" s="25"/>
       <c r="N8" s="25"/>
-      <c r="O8" s="28"/>
+      <c r="O8" s="26"/>
     </row>
     <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="24"/>
@@ -1392,19 +1392,19 @@
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="62">
+      <c r="G9" s="29"/>
+      <c r="H9" s="54">
         <v>29.654751000000001</v>
       </c>
-      <c r="I9" s="63">
+      <c r="I9" s="55">
         <v>24.414689200000002</v>
       </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25"/>
-      <c r="O9" s="28"/>
+      <c r="O9" s="26"/>
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="24"/>
@@ -1412,239 +1412,239 @@
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
-      <c r="G10" s="35"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
-      <c r="K10" s="35"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
-      <c r="O10" s="28"/>
+      <c r="O10" s="26"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="32" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
-      <c r="J11" s="53" t="s">
+      <c r="J11" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="32" t="s">
+      <c r="K11" s="28" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="28"/>
+      <c r="O11" s="26"/>
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="24"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="38">
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="34">
         <v>25.221986399999999</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="35">
         <v>21.527282199999998</v>
       </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
-      <c r="J12" s="38">
+      <c r="J12" s="34">
         <v>27.580023400000002</v>
       </c>
-      <c r="K12" s="39">
+      <c r="K12" s="35">
         <v>24.052491400000001</v>
       </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="28"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="26"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="24"/>
       <c r="C13" s="25"/>
-      <c r="D13" s="35"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="35"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
-      <c r="K13" s="35"/>
+      <c r="K13" s="31"/>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="28"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="26"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="24"/>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="32" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="25"/>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="50" t="s">
+      <c r="G14" s="46" t="s">
         <v>26</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="53" t="s">
+      <c r="J14" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="37" t="s">
         <v>32</v>
       </c>
       <c r="L14" s="25"/>
-      <c r="M14" s="54" t="s">
+      <c r="M14" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="32" t="s">
+      <c r="N14" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="O14" s="28"/>
+      <c r="O14" s="26"/>
     </row>
     <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="24"/>
-      <c r="C15" s="48">
+      <c r="C15" s="44">
         <v>20.513377200000001</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="40">
         <v>22.672564600000001</v>
       </c>
       <c r="E15" s="25"/>
-      <c r="F15" s="38">
+      <c r="F15" s="34">
         <v>27.053283400000002</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="35">
         <v>15.070951000000001</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
-      <c r="J15" s="38">
+      <c r="J15" s="34">
         <v>30.242114600000001</v>
       </c>
-      <c r="K15" s="39">
+      <c r="K15" s="35">
         <v>21.540104599999999</v>
       </c>
       <c r="L15" s="25"/>
-      <c r="M15" s="48">
+      <c r="M15" s="44">
         <v>21.9268486</v>
       </c>
-      <c r="N15" s="44">
+      <c r="N15" s="40">
         <v>24.780802000000001</v>
       </c>
-      <c r="O15" s="28"/>
+      <c r="O15" s="26"/>
     </row>
     <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
-      <c r="D16" s="35"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
-      <c r="G16" s="35"/>
+      <c r="G16" s="31"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
-      <c r="K16" s="35"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="28"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="26"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="24"/>
-      <c r="C17" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="49" t="s">
+      <c r="C17" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="45" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="25"/>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G17" s="46" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="52" t="s">
+      <c r="J17" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="K17" s="37" t="s">
         <v>32</v>
       </c>
       <c r="L17" s="25"/>
-      <c r="M17" s="37" t="s">
+      <c r="M17" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="55" t="s">
+      <c r="N17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="28"/>
+      <c r="O17" s="26"/>
     </row>
     <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="24"/>
-      <c r="C18" s="38">
+      <c r="C18" s="34">
         <v>24.019498599999999</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="35">
         <v>16.808707200000001</v>
       </c>
       <c r="E18" s="25"/>
-      <c r="F18" s="48">
+      <c r="F18" s="44">
         <v>17.630067400000001</v>
       </c>
-      <c r="G18" s="44">
+      <c r="G18" s="40">
         <v>21.191239599999999</v>
       </c>
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
-      <c r="J18" s="48">
+      <c r="J18" s="44">
         <v>24.766590399999998</v>
       </c>
-      <c r="K18" s="44">
+      <c r="K18" s="40">
         <v>24.890312600000001</v>
       </c>
       <c r="L18" s="25"/>
-      <c r="M18" s="38">
+      <c r="M18" s="34">
         <v>24.365172999999999</v>
       </c>
-      <c r="N18" s="51">
+      <c r="N18" s="47">
         <v>23.2420498</v>
       </c>
-      <c r="O18" s="28"/>
+      <c r="O18" s="26"/>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="47"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5286,8 +5286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAF23B6-5314-479B-B7E6-9EE40B3A92C0}">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6705,8 +6705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8808A2A0-A82D-4432-BDF5-AA68357B3978}">
   <dimension ref="A1:N222"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="H213" sqref="H213"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>